<commit_message>
planilla actualizada con nombres nuevos
</commit_message>
<xml_diff>
--- a/DB_RUST_1/soy_rust_original.xlsx
+++ b/DB_RUST_1/soy_rust_original.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="214">
   <si>
     <t xml:space="preserve">N°</t>
   </si>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">Daños Mecanicos</t>
   </si>
   <si>
-    <t xml:space="preserve">R2</t>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_56</t>
   </si>
   <si>
     <t xml:space="preserve">4032 x 3024</t>
@@ -88,583 +88,580 @@
     <t xml:space="preserve">No</t>
   </si>
   <si>
-    <t xml:space="preserve">R4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R42</t>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI₁</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_163</t>
   </si>
   <si>
     <t xml:space="preserve">-</t>
   </si>
   <si>
-    <t xml:space="preserve">R44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R74</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R86</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R88</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R92</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R98</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R108</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R116</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R122</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R124</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R126</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R130</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R134</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R136</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R140</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R142</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R144</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R146</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R148</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R152</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R154</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R156</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R158</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R160</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R162</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R164</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R166</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R168</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R170</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R172</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R174</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R176</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R178</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R180</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R182</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R184</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R186</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R190</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R192</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R194</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R196</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R198</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R202</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R204</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R208</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R212</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R214</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R216</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R218</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R224</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R226</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R228</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R230</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R232</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R236</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R238</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R240</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R242</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R244</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R246</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R248</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R256</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R258</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R260</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R262</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R264</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R266</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R268</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R270</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R272</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R274</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R276</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R278</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R280</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R282</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R284</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R286</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R288</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R290</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R292</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R294</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R296</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R298</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R304</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R306</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R308</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R310</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R312</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R314</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R316</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R318</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R320</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R322</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R324</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R326</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R328</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R330</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R332</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R334</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R336</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R338</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R340</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R342</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R344</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R346</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R348</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R350</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R352</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R354</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R356</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R358</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R360</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R362</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R364</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R366</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R368</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R370</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R372</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R374</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R376</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R378</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R380</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R382</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R384</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R386</t>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_191</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI₂</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI₃</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI₄</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI₅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI₆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI₇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI₈</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI₉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_03_10_AC_SOY_RUST_UCI_159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_12_23_AC_SOY_RUST_UCI_160</t>
   </si>
 </sst>
 </file>
@@ -675,7 +672,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -707,6 +704,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -805,7 +809,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -842,6 +846,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -870,7 +878,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -974,11 +982,11 @@
   <dimension ref="A1:O195"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1486" ySplit="960" topLeftCell="F169" activePane="topRight" state="split"/>
+      <pane xSplit="1224" ySplit="960" topLeftCell="A178" activePane="bottomRight" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N2" activeCellId="0" sqref="N2"/>
-      <selection pane="bottomLeft" activeCell="A169" activeCellId="0" sqref="A169"/>
-      <selection pane="bottomRight" activeCell="F169" activeCellId="0" sqref="F169"/>
+      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A178" activeCellId="0" sqref="A178"/>
+      <selection pane="bottomRight" activeCell="C196" activeCellId="0" sqref="C196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1197,7 +1205,7 @@
       <c r="A6" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="6" t="n">
@@ -1377,7 +1385,7 @@
       <c r="N9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="O9" s="10" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1523,49 +1531,49 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="n">
+      <c r="A13" s="11" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="11" t="n">
+      <c r="C13" s="12" t="n">
         <v>8</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="11" t="n">
+      <c r="D13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="12" t="n">
         <v>3.2</v>
       </c>
-      <c r="G13" s="11" t="n">
+      <c r="G13" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="H13" s="11" t="n">
+      <c r="H13" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="I13" s="13" t="n">
+      <c r="I13" s="14" t="n">
         <v>43168</v>
       </c>
-      <c r="J13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O13" s="11" t="s">
+      <c r="J13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1993,49 +2001,49 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" s="11" t="s">
+      <c r="A23" s="11" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="11" t="n">
+      <c r="C23" s="12" t="n">
         <v>8</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="11" t="n">
+      <c r="D23" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="12" t="n">
         <v>3.5</v>
       </c>
-      <c r="G23" s="11" t="n">
+      <c r="G23" s="12" t="n">
         <v>4.6</v>
       </c>
-      <c r="H23" s="12" t="s">
+      <c r="H23" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="I23" s="13" t="n">
+      <c r="I23" s="14" t="n">
         <v>43168</v>
       </c>
-      <c r="J23" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L23" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="M23" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="N23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O23" s="11" t="s">
+      <c r="J23" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3782,22 +3790,22 @@
       <c r="A61" s="5" t="n">
         <v>59</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C61" s="14" t="n">
+      <c r="C61" s="15" t="n">
         <v>55</v>
       </c>
-      <c r="D61" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E61" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F61" s="14" t="n">
+      <c r="D61" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" s="15" t="n">
         <v>5.3</v>
       </c>
-      <c r="G61" s="14" t="n">
+      <c r="G61" s="15" t="n">
         <v>10</v>
       </c>
       <c r="H61" s="6" t="n">
@@ -3876,22 +3884,22 @@
       <c r="A63" s="5" t="n">
         <v>61</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C63" s="14" t="n">
+      <c r="C63" s="15" t="n">
         <v>9</v>
       </c>
-      <c r="D63" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E63" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F63" s="14" t="n">
+      <c r="D63" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F63" s="15" t="n">
         <v>3.3</v>
       </c>
-      <c r="G63" s="14" t="n">
+      <c r="G63" s="15" t="n">
         <v>3.6</v>
       </c>
       <c r="H63" s="7" t="s">
@@ -3923,22 +3931,22 @@
       <c r="A64" s="5" t="n">
         <v>62</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C64" s="14" t="n">
+      <c r="C64" s="15" t="n">
         <v>55</v>
       </c>
-      <c r="D64" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E64" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F64" s="14" t="n">
+      <c r="D64" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" s="15" t="n">
         <v>6.9</v>
       </c>
-      <c r="G64" s="14" t="n">
+      <c r="G64" s="15" t="n">
         <v>12</v>
       </c>
       <c r="H64" s="6" t="n">
@@ -3970,22 +3978,22 @@
       <c r="A65" s="5" t="n">
         <v>63</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C65" s="14" t="n">
+      <c r="C65" s="15" t="n">
         <v>56</v>
       </c>
-      <c r="D65" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E65" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F65" s="14" t="n">
+      <c r="D65" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E65" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F65" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="G65" s="14" t="n">
+      <c r="G65" s="15" t="n">
         <v>15</v>
       </c>
       <c r="H65" s="6" t="n">
@@ -4064,22 +4072,22 @@
       <c r="A67" s="5" t="n">
         <v>65</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C67" s="14" t="n">
+      <c r="C67" s="15" t="n">
         <v>56</v>
       </c>
-      <c r="D67" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E67" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F67" s="14" t="n">
+      <c r="D67" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E67" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F67" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="G67" s="14" t="n">
+      <c r="G67" s="15" t="n">
         <v>9.2</v>
       </c>
       <c r="H67" s="6" t="n">
@@ -4299,22 +4307,22 @@
       <c r="A72" s="5" t="n">
         <v>70</v>
       </c>
-      <c r="B72" s="14" t="s">
+      <c r="B72" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C72" s="14" t="n">
+      <c r="C72" s="15" t="n">
         <v>58</v>
       </c>
-      <c r="D72" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E72" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F72" s="14" t="n">
+      <c r="D72" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E72" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F72" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="G72" s="14" t="n">
+      <c r="G72" s="15" t="n">
         <v>9</v>
       </c>
       <c r="H72" s="6" t="n">
@@ -4346,22 +4354,22 @@
       <c r="A73" s="5" t="n">
         <v>71</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B73" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C73" s="14" t="n">
+      <c r="C73" s="15" t="n">
         <v>58</v>
       </c>
-      <c r="D73" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E73" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F73" s="14" t="n">
+      <c r="D73" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E73" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F73" s="15" t="n">
         <v>4.9</v>
       </c>
-      <c r="G73" s="14" t="n">
+      <c r="G73" s="15" t="n">
         <v>11.2</v>
       </c>
       <c r="H73" s="6" t="n">
@@ -4393,22 +4401,22 @@
       <c r="A74" s="5" t="n">
         <v>72</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C74" s="14" t="n">
+      <c r="C74" s="15" t="n">
         <v>9</v>
       </c>
-      <c r="D74" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E74" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F74" s="14" t="n">
+      <c r="D74" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E74" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F74" s="15" t="n">
         <v>2.3</v>
       </c>
-      <c r="G74" s="14" t="n">
+      <c r="G74" s="15" t="n">
         <v>3.5</v>
       </c>
       <c r="H74" s="7" t="s">
@@ -4910,22 +4918,22 @@
       <c r="A85" s="5" t="n">
         <v>83</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B85" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C85" s="14" t="n">
+      <c r="C85" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="D85" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E85" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F85" s="14" t="n">
+      <c r="D85" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E85" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F85" s="15" t="n">
         <v>2.5</v>
       </c>
-      <c r="G85" s="14" t="n">
+      <c r="G85" s="15" t="n">
         <v>3.5</v>
       </c>
       <c r="H85" s="7" t="s">
@@ -5051,22 +5059,22 @@
       <c r="A88" s="5" t="n">
         <v>86</v>
       </c>
-      <c r="B88" s="14" t="s">
+      <c r="B88" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C88" s="14" t="n">
+      <c r="C88" s="15" t="n">
         <v>62</v>
       </c>
-      <c r="D88" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E88" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F88" s="14" t="n">
+      <c r="D88" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E88" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F88" s="15" t="n">
         <v>6.8</v>
       </c>
-      <c r="G88" s="14" t="n">
+      <c r="G88" s="15" t="n">
         <v>9.5</v>
       </c>
       <c r="H88" s="6" t="n">
@@ -5571,7 +5579,7 @@
       <c r="B99" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C99" s="16" t="n">
+      <c r="C99" s="17" t="n">
         <v>64</v>
       </c>
       <c r="D99" s="6" t="s">
@@ -6088,7 +6096,7 @@
       <c r="B110" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C110" s="17" t="n">
+      <c r="C110" s="18" t="n">
         <v>53</v>
       </c>
       <c r="D110" s="6" t="s">
@@ -6097,10 +6105,10 @@
       <c r="E110" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F110" s="17" t="n">
+      <c r="F110" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="G110" s="17" t="n">
+      <c r="G110" s="18" t="n">
         <v>8.8</v>
       </c>
       <c r="H110" s="6" t="n">
@@ -6135,7 +6143,7 @@
       <c r="B111" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C111" s="17" t="n">
+      <c r="C111" s="18" t="n">
         <v>56</v>
       </c>
       <c r="D111" s="6" t="s">
@@ -6144,10 +6152,10 @@
       <c r="E111" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F111" s="17" t="n">
+      <c r="F111" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="G111" s="17" t="n">
+      <c r="G111" s="18" t="n">
         <v>9</v>
       </c>
       <c r="H111" s="6" t="n">
@@ -6182,7 +6190,7 @@
       <c r="B112" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C112" s="17" t="n">
+      <c r="C112" s="18" t="n">
         <v>59</v>
       </c>
       <c r="D112" s="6" t="s">
@@ -6191,10 +6199,10 @@
       <c r="E112" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F112" s="17" t="n">
+      <c r="F112" s="18" t="n">
         <v>10.5</v>
       </c>
-      <c r="G112" s="17" t="n">
+      <c r="G112" s="18" t="n">
         <v>6.5</v>
       </c>
       <c r="H112" s="6" t="n">
@@ -6238,10 +6246,10 @@
       <c r="E113" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F113" s="17" t="n">
+      <c r="F113" s="18" t="n">
         <v>6.5</v>
       </c>
-      <c r="G113" s="17" t="n">
+      <c r="G113" s="18" t="n">
         <v>7.3</v>
       </c>
       <c r="H113" s="6" t="n">
@@ -6276,7 +6284,7 @@
       <c r="B114" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C114" s="17" t="n">
+      <c r="C114" s="18" t="n">
         <v>61</v>
       </c>
       <c r="D114" s="6" t="s">
@@ -6285,10 +6293,10 @@
       <c r="E114" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F114" s="17" t="n">
+      <c r="F114" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="G114" s="17" t="n">
+      <c r="G114" s="18" t="n">
         <v>8</v>
       </c>
       <c r="H114" s="6" t="n">
@@ -6323,7 +6331,7 @@
       <c r="B115" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C115" s="17" t="n">
+      <c r="C115" s="18" t="n">
         <v>67</v>
       </c>
       <c r="D115" s="6" t="s">
@@ -6332,10 +6340,10 @@
       <c r="E115" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F115" s="17" t="n">
+      <c r="F115" s="18" t="n">
         <v>6</v>
       </c>
-      <c r="G115" s="17" t="n">
+      <c r="G115" s="18" t="n">
         <v>8</v>
       </c>
       <c r="H115" s="6" t="n">
@@ -6370,7 +6378,7 @@
       <c r="B116" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C116" s="17" t="n">
+      <c r="C116" s="18" t="n">
         <v>67</v>
       </c>
       <c r="D116" s="6" t="s">
@@ -6379,10 +6387,10 @@
       <c r="E116" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F116" s="17" t="n">
+      <c r="F116" s="18" t="n">
         <v>5.2</v>
       </c>
-      <c r="G116" s="17" t="n">
+      <c r="G116" s="18" t="n">
         <v>7</v>
       </c>
       <c r="H116" s="6" t="n">
@@ -6417,7 +6425,7 @@
       <c r="B117" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C117" s="17" t="n">
+      <c r="C117" s="18" t="n">
         <v>67</v>
       </c>
       <c r="D117" s="6" t="s">
@@ -6426,10 +6434,10 @@
       <c r="E117" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F117" s="17" t="n">
+      <c r="F117" s="18" t="n">
         <v>6.5</v>
       </c>
-      <c r="G117" s="17" t="n">
+      <c r="G117" s="18" t="n">
         <v>8</v>
       </c>
       <c r="H117" s="6" t="n">
@@ -6511,7 +6519,7 @@
       <c r="B119" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C119" s="17" t="n">
+      <c r="C119" s="18" t="n">
         <v>68</v>
       </c>
       <c r="D119" s="6" t="s">
@@ -6520,10 +6528,10 @@
       <c r="E119" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F119" s="17" t="n">
+      <c r="F119" s="18" t="n">
         <v>6.2</v>
       </c>
-      <c r="G119" s="17" t="n">
+      <c r="G119" s="18" t="n">
         <v>9.5</v>
       </c>
       <c r="H119" s="6" t="n">
@@ -6558,7 +6566,7 @@
       <c r="B120" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C120" s="17" t="n">
+      <c r="C120" s="18" t="n">
         <v>68</v>
       </c>
       <c r="D120" s="6" t="s">
@@ -6567,10 +6575,10 @@
       <c r="E120" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F120" s="17" t="n">
+      <c r="F120" s="18" t="n">
         <v>6</v>
       </c>
-      <c r="G120" s="17" t="n">
+      <c r="G120" s="18" t="n">
         <v>9.8</v>
       </c>
       <c r="H120" s="6" t="n">
@@ -6605,7 +6613,7 @@
       <c r="B121" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C121" s="17" t="n">
+      <c r="C121" s="18" t="n">
         <v>68</v>
       </c>
       <c r="D121" s="6" t="s">
@@ -6614,10 +6622,10 @@
       <c r="E121" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F121" s="17" t="n">
+      <c r="F121" s="18" t="n">
         <v>6.3</v>
       </c>
-      <c r="G121" s="17" t="n">
+      <c r="G121" s="18" t="n">
         <v>8.3</v>
       </c>
       <c r="H121" s="6" t="n">
@@ -6652,7 +6660,7 @@
       <c r="B122" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C122" s="17" t="n">
+      <c r="C122" s="18" t="n">
         <v>68</v>
       </c>
       <c r="D122" s="6" t="s">
@@ -6661,10 +6669,10 @@
       <c r="E122" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F122" s="17" t="n">
+      <c r="F122" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="G122" s="17" t="n">
+      <c r="G122" s="18" t="n">
         <v>8</v>
       </c>
       <c r="H122" s="6" t="n">
@@ -6699,7 +6707,7 @@
       <c r="B123" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C123" s="17" t="n">
+      <c r="C123" s="18" t="n">
         <v>68</v>
       </c>
       <c r="D123" s="6" t="s">
@@ -6708,10 +6716,10 @@
       <c r="E123" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F123" s="17" t="n">
+      <c r="F123" s="18" t="n">
         <v>5.3</v>
       </c>
-      <c r="G123" s="17" t="n">
+      <c r="G123" s="18" t="n">
         <v>10</v>
       </c>
       <c r="H123" s="6" t="n">
@@ -6885,7 +6893,7 @@
         <v>125</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C127" s="6" t="n">
         <v>12</v>
@@ -6932,7 +6940,7 @@
         <v>126</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C128" s="6" t="n">
         <v>12</v>
@@ -6975,143 +6983,143 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="10" t="n">
+      <c r="A129" s="11" t="n">
         <v>127</v>
       </c>
-      <c r="B129" s="11" t="s">
+      <c r="B129" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C129" s="12" t="n">
+        <v>13</v>
+      </c>
+      <c r="D129" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E129" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F129" s="12" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="G129" s="12" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H129" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="I129" s="14" t="n">
+        <v>43091</v>
+      </c>
+      <c r="J129" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K129" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L129" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="M129" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="N129" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O129" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="11" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C129" s="11" t="n">
+      <c r="C130" s="12" t="n">
         <v>13</v>
       </c>
-      <c r="D129" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E129" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F129" s="11" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="G129" s="11" t="n">
+      <c r="D130" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E130" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F130" s="12" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="G130" s="12" t="n">
         <v>4.5</v>
       </c>
-      <c r="H129" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="I129" s="13" t="n">
+      <c r="H130" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="I130" s="14" t="n">
         <v>43091</v>
       </c>
-      <c r="J129" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K129" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="L129" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M129" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N129" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O129" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="10" t="n">
-        <v>128</v>
-      </c>
-      <c r="B130" s="11" t="s">
+      <c r="J130" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K130" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L130" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="M130" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="N130" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O130" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="11" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="C130" s="11" t="n">
+      <c r="C131" s="12" t="n">
         <v>13</v>
       </c>
-      <c r="D130" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E130" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F130" s="11" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="G130" s="11" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="H130" s="11" t="n">
+      <c r="D131" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E131" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F131" s="12" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G131" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="H131" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="I130" s="13" t="n">
+      <c r="I131" s="14" t="n">
         <v>43091</v>
       </c>
-      <c r="J130" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K130" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="L130" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M130" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N130" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O130" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="10" t="n">
-        <v>129</v>
-      </c>
-      <c r="B131" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="C131" s="11" t="n">
-        <v>13</v>
-      </c>
-      <c r="D131" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E131" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F131" s="11" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="G131" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="H131" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="I131" s="13" t="n">
-        <v>43091</v>
-      </c>
-      <c r="J131" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K131" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="L131" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M131" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N131" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O131" s="11" t="s">
+      <c r="J131" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K131" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L131" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="M131" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="N131" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O131" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -7120,7 +7128,7 @@
         <v>130</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C132" s="6" t="n">
         <v>14</v>
@@ -7167,7 +7175,7 @@
         <v>131</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C133" s="6" t="n">
         <v>14</v>
@@ -7214,7 +7222,7 @@
         <v>132</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C134" s="6" t="n">
         <v>14</v>
@@ -7261,7 +7269,7 @@
         <v>133</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C135" s="6" t="n">
         <v>15</v>
@@ -7308,7 +7316,7 @@
         <v>134</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C136" s="6" t="n">
         <v>15</v>
@@ -7355,7 +7363,7 @@
         <v>135</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C137" s="6" t="n">
         <v>15</v>
@@ -7402,7 +7410,7 @@
         <v>136</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C138" s="6" t="n">
         <v>16</v>
@@ -7449,7 +7457,7 @@
         <v>137</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C139" s="6" t="n">
         <v>16</v>
@@ -7496,7 +7504,7 @@
         <v>138</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C140" s="6" t="n">
         <v>16</v>
@@ -7543,7 +7551,7 @@
         <v>139</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C141" s="6" t="n">
         <v>17</v>
@@ -7590,7 +7598,7 @@
         <v>140</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C142" s="6" t="n">
         <v>17</v>
@@ -7637,7 +7645,7 @@
         <v>141</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C143" s="6" t="n">
         <v>17</v>
@@ -7684,7 +7692,7 @@
         <v>142</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C144" s="6" t="n">
         <v>18</v>
@@ -7731,7 +7739,7 @@
         <v>143</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C145" s="6" t="n">
         <v>18</v>
@@ -7778,7 +7786,7 @@
         <v>144</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C146" s="6" t="n">
         <v>18</v>
@@ -7825,7 +7833,7 @@
         <v>145</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C147" s="6" t="n">
         <v>19</v>
@@ -7872,7 +7880,7 @@
         <v>146</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C148" s="6" t="n">
         <v>19</v>
@@ -7919,7 +7927,7 @@
         <v>147</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C149" s="6" t="n">
         <v>19</v>
@@ -7966,7 +7974,7 @@
         <v>148</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C150" s="6" t="n">
         <v>20</v>
@@ -8013,7 +8021,7 @@
         <v>149</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C151" s="6" t="n">
         <v>20</v>
@@ -8060,7 +8068,7 @@
         <v>150</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C152" s="6" t="n">
         <v>20</v>
@@ -8107,7 +8115,7 @@
         <v>151</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C153" s="6" t="n">
         <v>21</v>
@@ -8154,7 +8162,7 @@
         <v>152</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C154" s="6" t="n">
         <v>21</v>
@@ -8201,7 +8209,7 @@
         <v>153</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C155" s="6" t="n">
         <v>21</v>
@@ -8248,7 +8256,7 @@
         <v>154</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C156" s="6" t="n">
         <v>22</v>
@@ -8295,7 +8303,7 @@
         <v>155</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C157" s="6" t="n">
         <v>22</v>
@@ -8342,7 +8350,7 @@
         <v>156</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C158" s="6" t="n">
         <v>22</v>
@@ -8389,7 +8397,7 @@
         <v>157</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C159" s="6" t="n">
         <v>23</v>
@@ -8436,7 +8444,7 @@
         <v>158</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C160" s="6" t="n">
         <v>23</v>
@@ -8483,7 +8491,7 @@
         <v>159</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C161" s="6" t="n">
         <v>24</v>
@@ -8530,7 +8538,7 @@
         <v>160</v>
       </c>
       <c r="B162" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C162" s="6" t="n">
         <v>24</v>
@@ -8577,7 +8585,7 @@
         <v>161</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C163" s="6" t="n">
         <v>24</v>
@@ -8624,7 +8632,7 @@
         <v>162</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C164" s="6" t="n">
         <v>24</v>
@@ -8671,7 +8679,7 @@
         <v>163</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C165" s="6" t="n">
         <v>25</v>
@@ -8718,7 +8726,7 @@
         <v>164</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C166" s="6" t="n">
         <v>25</v>
@@ -8765,7 +8773,7 @@
         <v>165</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C167" s="6" t="n">
         <v>25</v>
@@ -8812,7 +8820,7 @@
         <v>166</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C168" s="6" t="n">
         <v>26</v>
@@ -8859,7 +8867,7 @@
         <v>167</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C169" s="6" t="n">
         <v>26</v>
@@ -8906,7 +8914,7 @@
         <v>168</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C170" s="6" t="n">
         <v>26</v>
@@ -8926,7 +8934,7 @@
       <c r="H170" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="I170" s="18" t="n">
+      <c r="I170" s="19" t="n">
         <v>43092</v>
       </c>
       <c r="J170" s="7" t="s">
@@ -8953,7 +8961,7 @@
         <v>169</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C171" s="6" t="n">
         <v>27</v>
@@ -8973,7 +8981,7 @@
       <c r="H171" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="I171" s="18" t="n">
+      <c r="I171" s="19" t="n">
         <v>43092</v>
       </c>
       <c r="J171" s="7" t="s">
@@ -9000,7 +9008,7 @@
         <v>170</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C172" s="6" t="n">
         <v>27</v>
@@ -9020,7 +9028,7 @@
       <c r="H172" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I172" s="18" t="n">
+      <c r="I172" s="19" t="n">
         <v>43092</v>
       </c>
       <c r="J172" s="7" t="s">
@@ -9047,7 +9055,7 @@
         <v>171</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C173" s="6" t="n">
         <v>27</v>
@@ -9067,7 +9075,7 @@
       <c r="H173" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="I173" s="18" t="n">
+      <c r="I173" s="19" t="n">
         <v>43092</v>
       </c>
       <c r="J173" s="7" t="s">
@@ -9093,28 +9101,28 @@
       <c r="A174" s="5" t="n">
         <v>172</v>
       </c>
-      <c r="B174" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="C174" s="19" t="n">
+      <c r="B174" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="C174" s="20" t="n">
         <v>27</v>
       </c>
-      <c r="D174" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E174" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F174" s="19" t="n">
+      <c r="D174" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E174" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F174" s="20" t="n">
         <v>3.5</v>
       </c>
-      <c r="G174" s="19" t="n">
+      <c r="G174" s="20" t="n">
         <v>4.4</v>
       </c>
-      <c r="H174" s="20" t="s">
+      <c r="H174" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="I174" s="21" t="n">
+      <c r="I174" s="22" t="n">
         <v>42802</v>
       </c>
       <c r="J174" s="7" t="s">
@@ -9141,7 +9149,7 @@
         <v>173</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C175" s="6" t="n">
         <v>28</v>
@@ -9161,7 +9169,7 @@
       <c r="H175" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I175" s="18" t="n">
+      <c r="I175" s="19" t="n">
         <v>43092</v>
       </c>
       <c r="J175" s="7" t="s">
@@ -9188,7 +9196,7 @@
         <v>174</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C176" s="6" t="n">
         <v>28</v>
@@ -9208,7 +9216,7 @@
       <c r="H176" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I176" s="18" t="n">
+      <c r="I176" s="19" t="n">
         <v>43092</v>
       </c>
       <c r="J176" s="7" t="s">
@@ -9235,7 +9243,7 @@
         <v>175</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C177" s="6" t="n">
         <v>28</v>
@@ -9255,7 +9263,7 @@
       <c r="H177" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I177" s="18" t="n">
+      <c r="I177" s="19" t="n">
         <v>43092</v>
       </c>
       <c r="J177" s="7" t="s">
@@ -9282,7 +9290,7 @@
         <v>176</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C178" s="6" t="n">
         <v>29</v>
@@ -9302,7 +9310,7 @@
       <c r="H178" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="I178" s="18" t="n">
+      <c r="I178" s="19" t="n">
         <v>43092</v>
       </c>
       <c r="J178" s="7" t="s">
@@ -9329,7 +9337,7 @@
         <v>177</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C179" s="6" t="n">
         <v>29</v>
@@ -9349,7 +9357,7 @@
       <c r="H179" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="I179" s="18" t="n">
+      <c r="I179" s="19" t="n">
         <v>43092</v>
       </c>
       <c r="J179" s="7" t="s">
@@ -9376,7 +9384,7 @@
         <v>178</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C180" s="6" t="n">
         <v>30</v>
@@ -9396,7 +9404,7 @@
       <c r="H180" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I180" s="18" t="n">
+      <c r="I180" s="19" t="n">
         <v>43092</v>
       </c>
       <c r="J180" s="7" t="s">
@@ -9423,7 +9431,7 @@
         <v>179</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C181" s="6" t="n">
         <v>30</v>
@@ -9443,7 +9451,7 @@
       <c r="H181" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I181" s="18" t="n">
+      <c r="I181" s="19" t="n">
         <v>43092</v>
       </c>
       <c r="J181" s="7" t="s">
@@ -9470,7 +9478,7 @@
         <v>180</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C182" s="6" t="n">
         <v>30</v>
@@ -9490,7 +9498,7 @@
       <c r="H182" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="I182" s="18" t="n">
+      <c r="I182" s="19" t="n">
         <v>43092</v>
       </c>
       <c r="J182" s="7" t="s">
@@ -9517,7 +9525,7 @@
         <v>181</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C183" s="6" t="n">
         <v>31</v>
@@ -9537,7 +9545,7 @@
       <c r="H183" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I183" s="18" t="n">
+      <c r="I183" s="19" t="n">
         <v>43092</v>
       </c>
       <c r="J183" s="7" t="s">
@@ -9564,7 +9572,7 @@
         <v>182</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C184" s="6" t="n">
         <v>31</v>
@@ -9584,7 +9592,7 @@
       <c r="H184" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="I184" s="18" t="n">
+      <c r="I184" s="19" t="n">
         <v>43092</v>
       </c>
       <c r="J184" s="7" t="s">
@@ -9611,7 +9619,7 @@
         <v>183</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C185" s="6" t="n">
         <v>31</v>
@@ -9631,7 +9639,7 @@
       <c r="H185" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="I185" s="18" t="n">
+      <c r="I185" s="19" t="n">
         <v>43092</v>
       </c>
       <c r="J185" s="7" t="s">
@@ -9658,7 +9666,7 @@
         <v>184</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C186" s="6" t="n">
         <v>32</v>
@@ -9705,7 +9713,7 @@
         <v>185</v>
       </c>
       <c r="B187" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C187" s="6" t="n">
         <v>32</v>
@@ -9752,7 +9760,7 @@
         <v>186</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C188" s="6" t="n">
         <v>33</v>
@@ -9799,7 +9807,7 @@
         <v>187</v>
       </c>
       <c r="B189" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C189" s="6" t="n">
         <v>33</v>
@@ -9846,7 +9854,7 @@
         <v>188</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C190" s="6" t="n">
         <v>33</v>
@@ -9893,7 +9901,7 @@
         <v>189</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C191" s="6" t="n">
         <v>35</v>
@@ -9940,7 +9948,7 @@
         <v>190</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C192" s="6" t="n">
         <v>35</v>
@@ -9987,7 +9995,7 @@
         <v>191</v>
       </c>
       <c r="B193" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C193" s="6" t="n">
         <v>35</v>
@@ -10034,7 +10042,7 @@
         <v>192</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C194" s="6" t="n">
         <v>36</v>
@@ -10081,7 +10089,7 @@
         <v>193</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C195" s="6" t="n">
         <v>7</v>

</xml_diff>

<commit_message>
planilla con nombres y enfermedades de bd de roya asiatica
</commit_message>
<xml_diff>
--- a/DB_RUST_1/soy_rust_original.xlsx
+++ b/DB_RUST_1/soy_rust_original.xlsx
@@ -672,7 +672,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -704,13 +704,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -809,7 +802,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -846,10 +839,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -878,7 +867,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -982,16 +971,29 @@
   <dimension ref="A1:O195"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1224" ySplit="960" topLeftCell="A178" activePane="bottomRight" state="split"/>
+      <pane xSplit="1078" ySplit="960" topLeftCell="A43" activePane="bottomRight" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A178" activeCellId="0" sqref="A178"/>
-      <selection pane="bottomRight" activeCell="C196" activeCellId="0" sqref="C196"/>
+      <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+      <selection pane="bottomRight" activeCell="L56" activeCellId="0" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="5.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="7.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1205,7 +1207,7 @@
       <c r="A6" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="6" t="n">
@@ -1385,7 +1387,7 @@
       <c r="N9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="O9" s="10" t="s">
+      <c r="O9" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1531,49 +1533,49 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="n">
+      <c r="A13" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="12" t="n">
+      <c r="C13" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="12" t="n">
+      <c r="D13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="11" t="n">
         <v>3.2</v>
       </c>
-      <c r="G13" s="12" t="n">
+      <c r="G13" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="H13" s="12" t="n">
+      <c r="H13" s="11" t="n">
         <v>7</v>
       </c>
-      <c r="I13" s="14" t="n">
+      <c r="I13" s="13" t="n">
         <v>43168</v>
       </c>
-      <c r="J13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="O13" s="12" t="s">
+      <c r="J13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1847,7 +1849,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M19" s="6" t="s">
         <v>21</v>
@@ -2001,49 +2003,49 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" s="12" t="s">
+      <c r="A23" s="10" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="12" t="n">
+      <c r="C23" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="12" t="n">
+      <c r="D23" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="11" t="n">
         <v>3.5</v>
       </c>
-      <c r="G23" s="12" t="n">
+      <c r="G23" s="11" t="n">
         <v>4.6</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="H23" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="I23" s="14" t="n">
+      <c r="I23" s="13" t="n">
         <v>43168</v>
       </c>
-      <c r="J23" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K23" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L23" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M23" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N23" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="O23" s="12" t="s">
+      <c r="J23" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23" s="11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2599,7 +2601,7 @@
         <v>20</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M35" s="6" t="s">
         <v>21</v>
@@ -3586,7 +3588,7 @@
         <v>20</v>
       </c>
       <c r="L56" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M56" s="6" t="s">
         <v>21</v>
@@ -3790,22 +3792,22 @@
       <c r="A61" s="5" t="n">
         <v>59</v>
       </c>
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C61" s="15" t="n">
+      <c r="C61" s="14" t="n">
         <v>55</v>
       </c>
-      <c r="D61" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E61" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F61" s="15" t="n">
+      <c r="D61" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" s="14" t="n">
         <v>5.3</v>
       </c>
-      <c r="G61" s="15" t="n">
+      <c r="G61" s="14" t="n">
         <v>10</v>
       </c>
       <c r="H61" s="6" t="n">
@@ -3884,22 +3886,22 @@
       <c r="A63" s="5" t="n">
         <v>61</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B63" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C63" s="15" t="n">
+      <c r="C63" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="D63" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E63" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F63" s="15" t="n">
+      <c r="D63" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F63" s="14" t="n">
         <v>3.3</v>
       </c>
-      <c r="G63" s="15" t="n">
+      <c r="G63" s="14" t="n">
         <v>3.6</v>
       </c>
       <c r="H63" s="7" t="s">
@@ -3931,22 +3933,22 @@
       <c r="A64" s="5" t="n">
         <v>62</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C64" s="15" t="n">
+      <c r="C64" s="14" t="n">
         <v>55</v>
       </c>
-      <c r="D64" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E64" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F64" s="15" t="n">
+      <c r="D64" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" s="14" t="n">
         <v>6.9</v>
       </c>
-      <c r="G64" s="15" t="n">
+      <c r="G64" s="14" t="n">
         <v>12</v>
       </c>
       <c r="H64" s="6" t="n">
@@ -3978,22 +3980,22 @@
       <c r="A65" s="5" t="n">
         <v>63</v>
       </c>
-      <c r="B65" s="15" t="s">
+      <c r="B65" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C65" s="15" t="n">
+      <c r="C65" s="14" t="n">
         <v>56</v>
       </c>
-      <c r="D65" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E65" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F65" s="15" t="n">
+      <c r="D65" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E65" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F65" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="G65" s="15" t="n">
+      <c r="G65" s="14" t="n">
         <v>15</v>
       </c>
       <c r="H65" s="6" t="n">
@@ -4072,22 +4074,22 @@
       <c r="A67" s="5" t="n">
         <v>65</v>
       </c>
-      <c r="B67" s="15" t="s">
+      <c r="B67" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C67" s="15" t="n">
+      <c r="C67" s="14" t="n">
         <v>56</v>
       </c>
-      <c r="D67" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E67" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F67" s="15" t="n">
+      <c r="D67" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E67" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F67" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="G67" s="15" t="n">
+      <c r="G67" s="14" t="n">
         <v>9.2</v>
       </c>
       <c r="H67" s="6" t="n">
@@ -4307,22 +4309,22 @@
       <c r="A72" s="5" t="n">
         <v>70</v>
       </c>
-      <c r="B72" s="15" t="s">
+      <c r="B72" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C72" s="15" t="n">
+      <c r="C72" s="14" t="n">
         <v>58</v>
       </c>
-      <c r="D72" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E72" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F72" s="15" t="n">
+      <c r="D72" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E72" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F72" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="G72" s="15" t="n">
+      <c r="G72" s="14" t="n">
         <v>9</v>
       </c>
       <c r="H72" s="6" t="n">
@@ -4354,22 +4356,22 @@
       <c r="A73" s="5" t="n">
         <v>71</v>
       </c>
-      <c r="B73" s="15" t="s">
+      <c r="B73" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C73" s="15" t="n">
+      <c r="C73" s="14" t="n">
         <v>58</v>
       </c>
-      <c r="D73" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E73" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F73" s="15" t="n">
+      <c r="D73" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E73" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F73" s="14" t="n">
         <v>4.9</v>
       </c>
-      <c r="G73" s="15" t="n">
+      <c r="G73" s="14" t="n">
         <v>11.2</v>
       </c>
       <c r="H73" s="6" t="n">
@@ -4401,22 +4403,22 @@
       <c r="A74" s="5" t="n">
         <v>72</v>
       </c>
-      <c r="B74" s="15" t="s">
+      <c r="B74" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C74" s="15" t="n">
+      <c r="C74" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="D74" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E74" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F74" s="15" t="n">
+      <c r="D74" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E74" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F74" s="14" t="n">
         <v>2.3</v>
       </c>
-      <c r="G74" s="15" t="n">
+      <c r="G74" s="14" t="n">
         <v>3.5</v>
       </c>
       <c r="H74" s="7" t="s">
@@ -4918,22 +4920,22 @@
       <c r="A85" s="5" t="n">
         <v>83</v>
       </c>
-      <c r="B85" s="15" t="s">
+      <c r="B85" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="C85" s="15" t="n">
+      <c r="C85" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="D85" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E85" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F85" s="15" t="n">
+      <c r="D85" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F85" s="14" t="n">
         <v>2.5</v>
       </c>
-      <c r="G85" s="15" t="n">
+      <c r="G85" s="14" t="n">
         <v>3.5</v>
       </c>
       <c r="H85" s="7" t="s">
@@ -5059,22 +5061,22 @@
       <c r="A88" s="5" t="n">
         <v>86</v>
       </c>
-      <c r="B88" s="15" t="s">
+      <c r="B88" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C88" s="15" t="n">
+      <c r="C88" s="14" t="n">
         <v>62</v>
       </c>
-      <c r="D88" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E88" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F88" s="15" t="n">
+      <c r="D88" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E88" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F88" s="14" t="n">
         <v>6.8</v>
       </c>
-      <c r="G88" s="15" t="n">
+      <c r="G88" s="14" t="n">
         <v>9.5</v>
       </c>
       <c r="H88" s="6" t="n">
@@ -5579,7 +5581,7 @@
       <c r="B99" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C99" s="17" t="n">
+      <c r="C99" s="16" t="n">
         <v>64</v>
       </c>
       <c r="D99" s="6" t="s">
@@ -6096,7 +6098,7 @@
       <c r="B110" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C110" s="18" t="n">
+      <c r="C110" s="17" t="n">
         <v>53</v>
       </c>
       <c r="D110" s="6" t="s">
@@ -6105,10 +6107,10 @@
       <c r="E110" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F110" s="18" t="n">
+      <c r="F110" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="G110" s="18" t="n">
+      <c r="G110" s="17" t="n">
         <v>8.8</v>
       </c>
       <c r="H110" s="6" t="n">
@@ -6143,7 +6145,7 @@
       <c r="B111" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C111" s="18" t="n">
+      <c r="C111" s="17" t="n">
         <v>56</v>
       </c>
       <c r="D111" s="6" t="s">
@@ -6152,10 +6154,10 @@
       <c r="E111" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F111" s="18" t="n">
+      <c r="F111" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="G111" s="18" t="n">
+      <c r="G111" s="17" t="n">
         <v>9</v>
       </c>
       <c r="H111" s="6" t="n">
@@ -6190,7 +6192,7 @@
       <c r="B112" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C112" s="18" t="n">
+      <c r="C112" s="17" t="n">
         <v>59</v>
       </c>
       <c r="D112" s="6" t="s">
@@ -6199,10 +6201,10 @@
       <c r="E112" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F112" s="18" t="n">
+      <c r="F112" s="17" t="n">
         <v>10.5</v>
       </c>
-      <c r="G112" s="18" t="n">
+      <c r="G112" s="17" t="n">
         <v>6.5</v>
       </c>
       <c r="H112" s="6" t="n">
@@ -6246,10 +6248,10 @@
       <c r="E113" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F113" s="18" t="n">
+      <c r="F113" s="17" t="n">
         <v>6.5</v>
       </c>
-      <c r="G113" s="18" t="n">
+      <c r="G113" s="17" t="n">
         <v>7.3</v>
       </c>
       <c r="H113" s="6" t="n">
@@ -6284,7 +6286,7 @@
       <c r="B114" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C114" s="18" t="n">
+      <c r="C114" s="17" t="n">
         <v>61</v>
       </c>
       <c r="D114" s="6" t="s">
@@ -6293,10 +6295,10 @@
       <c r="E114" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F114" s="18" t="n">
+      <c r="F114" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="G114" s="18" t="n">
+      <c r="G114" s="17" t="n">
         <v>8</v>
       </c>
       <c r="H114" s="6" t="n">
@@ -6331,7 +6333,7 @@
       <c r="B115" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C115" s="18" t="n">
+      <c r="C115" s="17" t="n">
         <v>67</v>
       </c>
       <c r="D115" s="6" t="s">
@@ -6340,10 +6342,10 @@
       <c r="E115" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F115" s="18" t="n">
+      <c r="F115" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="G115" s="18" t="n">
+      <c r="G115" s="17" t="n">
         <v>8</v>
       </c>
       <c r="H115" s="6" t="n">
@@ -6378,7 +6380,7 @@
       <c r="B116" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C116" s="18" t="n">
+      <c r="C116" s="17" t="n">
         <v>67</v>
       </c>
       <c r="D116" s="6" t="s">
@@ -6387,10 +6389,10 @@
       <c r="E116" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F116" s="18" t="n">
+      <c r="F116" s="17" t="n">
         <v>5.2</v>
       </c>
-      <c r="G116" s="18" t="n">
+      <c r="G116" s="17" t="n">
         <v>7</v>
       </c>
       <c r="H116" s="6" t="n">
@@ -6425,7 +6427,7 @@
       <c r="B117" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C117" s="18" t="n">
+      <c r="C117" s="17" t="n">
         <v>67</v>
       </c>
       <c r="D117" s="6" t="s">
@@ -6434,10 +6436,10 @@
       <c r="E117" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F117" s="18" t="n">
+      <c r="F117" s="17" t="n">
         <v>6.5</v>
       </c>
-      <c r="G117" s="18" t="n">
+      <c r="G117" s="17" t="n">
         <v>8</v>
       </c>
       <c r="H117" s="6" t="n">
@@ -6519,7 +6521,7 @@
       <c r="B119" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C119" s="18" t="n">
+      <c r="C119" s="17" t="n">
         <v>68</v>
       </c>
       <c r="D119" s="6" t="s">
@@ -6528,10 +6530,10 @@
       <c r="E119" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F119" s="18" t="n">
+      <c r="F119" s="17" t="n">
         <v>6.2</v>
       </c>
-      <c r="G119" s="18" t="n">
+      <c r="G119" s="17" t="n">
         <v>9.5</v>
       </c>
       <c r="H119" s="6" t="n">
@@ -6566,7 +6568,7 @@
       <c r="B120" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C120" s="18" t="n">
+      <c r="C120" s="17" t="n">
         <v>68</v>
       </c>
       <c r="D120" s="6" t="s">
@@ -6575,10 +6577,10 @@
       <c r="E120" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F120" s="18" t="n">
+      <c r="F120" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="G120" s="18" t="n">
+      <c r="G120" s="17" t="n">
         <v>9.8</v>
       </c>
       <c r="H120" s="6" t="n">
@@ -6613,7 +6615,7 @@
       <c r="B121" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C121" s="18" t="n">
+      <c r="C121" s="17" t="n">
         <v>68</v>
       </c>
       <c r="D121" s="6" t="s">
@@ -6622,10 +6624,10 @@
       <c r="E121" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F121" s="18" t="n">
+      <c r="F121" s="17" t="n">
         <v>6.3</v>
       </c>
-      <c r="G121" s="18" t="n">
+      <c r="G121" s="17" t="n">
         <v>8.3</v>
       </c>
       <c r="H121" s="6" t="n">
@@ -6660,7 +6662,7 @@
       <c r="B122" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C122" s="18" t="n">
+      <c r="C122" s="17" t="n">
         <v>68</v>
       </c>
       <c r="D122" s="6" t="s">
@@ -6669,10 +6671,10 @@
       <c r="E122" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F122" s="18" t="n">
+      <c r="F122" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="G122" s="18" t="n">
+      <c r="G122" s="17" t="n">
         <v>8</v>
       </c>
       <c r="H122" s="6" t="n">
@@ -6707,7 +6709,7 @@
       <c r="B123" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C123" s="18" t="n">
+      <c r="C123" s="17" t="n">
         <v>68</v>
       </c>
       <c r="D123" s="6" t="s">
@@ -6716,10 +6718,10 @@
       <c r="E123" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F123" s="18" t="n">
+      <c r="F123" s="17" t="n">
         <v>5.3</v>
       </c>
-      <c r="G123" s="18" t="n">
+      <c r="G123" s="17" t="n">
         <v>10</v>
       </c>
       <c r="H123" s="6" t="n">
@@ -6983,143 +6985,143 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="11" t="n">
+      <c r="A129" s="10" t="n">
         <v>127</v>
       </c>
-      <c r="B129" s="12" t="s">
+      <c r="B129" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="C129" s="12" t="n">
+      <c r="C129" s="11" t="n">
         <v>13</v>
       </c>
-      <c r="D129" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E129" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F129" s="12" t="n">
+      <c r="D129" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E129" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F129" s="11" t="n">
         <v>3.2</v>
       </c>
-      <c r="G129" s="12" t="n">
+      <c r="G129" s="11" t="n">
         <v>4.5</v>
       </c>
-      <c r="H129" s="12" t="n">
+      <c r="H129" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="I129" s="14" t="n">
+      <c r="I129" s="13" t="n">
         <v>43091</v>
       </c>
-      <c r="J129" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K129" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L129" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="M129" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="N129" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="O129" s="12" t="s">
+      <c r="J129" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K129" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L129" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M129" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N129" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O129" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="11" t="n">
+      <c r="A130" s="10" t="n">
         <v>128</v>
       </c>
-      <c r="B130" s="12" t="s">
+      <c r="B130" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="C130" s="12" t="n">
+      <c r="C130" s="11" t="n">
         <v>13</v>
       </c>
-      <c r="D130" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E130" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F130" s="12" t="n">
+      <c r="D130" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E130" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F130" s="11" t="n">
         <v>3.6</v>
       </c>
-      <c r="G130" s="12" t="n">
+      <c r="G130" s="11" t="n">
         <v>4.5</v>
       </c>
-      <c r="H130" s="12" t="n">
+      <c r="H130" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="I130" s="14" t="n">
+      <c r="I130" s="13" t="n">
         <v>43091</v>
       </c>
-      <c r="J130" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K130" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L130" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="M130" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="N130" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="O130" s="12" t="s">
+      <c r="J130" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K130" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L130" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M130" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N130" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O130" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="11" t="n">
+      <c r="A131" s="10" t="n">
         <v>129</v>
       </c>
-      <c r="B131" s="12" t="s">
+      <c r="B131" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C131" s="12" t="n">
+      <c r="C131" s="11" t="n">
         <v>13</v>
       </c>
-      <c r="D131" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E131" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F131" s="12" t="n">
+      <c r="D131" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E131" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F131" s="11" t="n">
         <v>3.5</v>
       </c>
-      <c r="G131" s="12" t="n">
+      <c r="G131" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="H131" s="12" t="n">
+      <c r="H131" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="I131" s="14" t="n">
+      <c r="I131" s="13" t="n">
         <v>43091</v>
       </c>
-      <c r="J131" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K131" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L131" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="M131" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="N131" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="O131" s="12" t="s">
+      <c r="J131" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K131" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L131" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M131" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N131" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O131" s="11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -8934,7 +8936,7 @@
       <c r="H170" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="I170" s="19" t="n">
+      <c r="I170" s="18" t="n">
         <v>43092</v>
       </c>
       <c r="J170" s="7" t="s">
@@ -8981,7 +8983,7 @@
       <c r="H171" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="I171" s="19" t="n">
+      <c r="I171" s="18" t="n">
         <v>43092</v>
       </c>
       <c r="J171" s="7" t="s">
@@ -9028,7 +9030,7 @@
       <c r="H172" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I172" s="19" t="n">
+      <c r="I172" s="18" t="n">
         <v>43092</v>
       </c>
       <c r="J172" s="7" t="s">
@@ -9075,7 +9077,7 @@
       <c r="H173" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="I173" s="19" t="n">
+      <c r="I173" s="18" t="n">
         <v>43092</v>
       </c>
       <c r="J173" s="7" t="s">
@@ -9101,28 +9103,28 @@
       <c r="A174" s="5" t="n">
         <v>172</v>
       </c>
-      <c r="B174" s="20" t="s">
+      <c r="B174" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="C174" s="20" t="n">
+      <c r="C174" s="19" t="n">
         <v>27</v>
       </c>
-      <c r="D174" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E174" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F174" s="20" t="n">
+      <c r="D174" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E174" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F174" s="19" t="n">
         <v>3.5</v>
       </c>
-      <c r="G174" s="20" t="n">
+      <c r="G174" s="19" t="n">
         <v>4.4</v>
       </c>
-      <c r="H174" s="21" t="s">
+      <c r="H174" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="I174" s="22" t="n">
+      <c r="I174" s="21" t="n">
         <v>42802</v>
       </c>
       <c r="J174" s="7" t="s">
@@ -9169,7 +9171,7 @@
       <c r="H175" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I175" s="19" t="n">
+      <c r="I175" s="18" t="n">
         <v>43092</v>
       </c>
       <c r="J175" s="7" t="s">
@@ -9216,7 +9218,7 @@
       <c r="H176" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I176" s="19" t="n">
+      <c r="I176" s="18" t="n">
         <v>43092</v>
       </c>
       <c r="J176" s="7" t="s">
@@ -9263,7 +9265,7 @@
       <c r="H177" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I177" s="19" t="n">
+      <c r="I177" s="18" t="n">
         <v>43092</v>
       </c>
       <c r="J177" s="7" t="s">
@@ -9310,7 +9312,7 @@
       <c r="H178" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="I178" s="19" t="n">
+      <c r="I178" s="18" t="n">
         <v>43092</v>
       </c>
       <c r="J178" s="7" t="s">
@@ -9357,7 +9359,7 @@
       <c r="H179" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="I179" s="19" t="n">
+      <c r="I179" s="18" t="n">
         <v>43092</v>
       </c>
       <c r="J179" s="7" t="s">
@@ -9404,7 +9406,7 @@
       <c r="H180" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I180" s="19" t="n">
+      <c r="I180" s="18" t="n">
         <v>43092</v>
       </c>
       <c r="J180" s="7" t="s">
@@ -9451,7 +9453,7 @@
       <c r="H181" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I181" s="19" t="n">
+      <c r="I181" s="18" t="n">
         <v>43092</v>
       </c>
       <c r="J181" s="7" t="s">
@@ -9498,7 +9500,7 @@
       <c r="H182" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="I182" s="19" t="n">
+      <c r="I182" s="18" t="n">
         <v>43092</v>
       </c>
       <c r="J182" s="7" t="s">
@@ -9545,7 +9547,7 @@
       <c r="H183" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I183" s="19" t="n">
+      <c r="I183" s="18" t="n">
         <v>43092</v>
       </c>
       <c r="J183" s="7" t="s">
@@ -9592,7 +9594,7 @@
       <c r="H184" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="I184" s="19" t="n">
+      <c r="I184" s="18" t="n">
         <v>43092</v>
       </c>
       <c r="J184" s="7" t="s">
@@ -9639,7 +9641,7 @@
       <c r="H185" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="I185" s="19" t="n">
+      <c r="I185" s="18" t="n">
         <v>43092</v>
       </c>
       <c r="J185" s="7" t="s">
@@ -10146,7 +10148,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="14" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>